<commit_message>
Updated excel sheet & testcase with additional function to include glitch user
</commit_message>
<xml_diff>
--- a/Python/POC__Automation 2.0/DDT/testdata.xlsx
+++ b/Python/POC__Automation 2.0/DDT/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -65,13 +65,16 @@
   </si>
   <si>
     <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -83,13 +86,24 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="&quot;DM Mono&quot;"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF132322"/>
+        <bgColor rgb="FF132322"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,11 +112,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -387,6 +404,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>